<commit_message>
Update results testing notes
</commit_message>
<xml_diff>
--- a/docs/xlsx/results_testing.xlsx
+++ b/docs/xlsx/results_testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\wsw-results\docs\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1444DD96-8FFF-441A-9ED4-7C3BF05C8052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD510C3E-0990-4414-B7F5-8037338DD9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D7D7223F-B91D-48E1-BDEF-EDFA67C005FF}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
   <si>
     <t>Course</t>
   </si>
@@ -77,6 +77,27 @@
   </si>
   <si>
     <t>* 200m / 500m courses seperately *</t>
+  </si>
+  <si>
+    <t>Alternative course lengths</t>
+  </si>
+  <si>
+    <t>Details missing from results</t>
+  </si>
+  <si>
+    <t>No results, only rundata</t>
+  </si>
+  <si>
+    <t>Craft types unspecified, some days</t>
+  </si>
+  <si>
+    <t>Categories unspecified</t>
+  </si>
+  <si>
+    <t>Categories + craft types unspecified</t>
+  </si>
+  <si>
+    <t>Categories + craft types unspecified on last day</t>
   </si>
 </sst>
 </file>
@@ -138,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -167,6 +188,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -483,18 +510,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB51FCCB-C3F0-44F1-8827-22234CF19BDE}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="34.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
@@ -507,9 +537,14 @@
       <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1998</v>
       </c>
@@ -525,11 +560,11 @@
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1999</v>
       </c>
@@ -546,7 +581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2000</v>
       </c>
@@ -562,11 +597,11 @@
       <c r="E4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2001</v>
       </c>
@@ -582,11 +617,14 @@
       <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2002</v>
       </c>
@@ -603,7 +641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2003</v>
       </c>
@@ -620,7 +658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2004</v>
       </c>
@@ -637,7 +675,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2005</v>
       </c>
@@ -653,8 +691,11 @@
       <c r="E9" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2006</v>
       </c>
@@ -670,8 +711,11 @@
       <c r="E10" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2007</v>
       </c>
@@ -688,24 +732,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2008</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2009</v>
       </c>
@@ -721,18 +765,21 @@
       <c r="E13" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2012</v>
       </c>

</xml_diff>

<commit_message>
Add note about names missing in 1998 results
</commit_message>
<xml_diff>
--- a/docs/xlsx/results_testing.xlsx
+++ b/docs/xlsx/results_testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\wsw-results\docs\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68959057-8A19-4818-8D48-9FEC44FAED30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C3F3F6-6A8D-4B8D-B781-80DD17E32D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D7D7223F-B91D-48E1-BDEF-EDFA67C005FF}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>Course</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Full list of runs only, not rankings</t>
+  </si>
+  <si>
+    <t>Event results do not show names</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +554,7 @@
       <c r="A2">
         <v>1998</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -561,7 +564,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>6</v>

</xml_diff>